<commit_message>
Update stand-up meeting template.
Create and update daily stand-up meeting template.
</commit_message>
<xml_diff>
--- a/Project_Files/GDP-02-Sprint05/Stand-up Meeting Sec03Team05 Sprint04.xlsx
+++ b/Project_Files/GDP-02-Sprint05/Stand-up Meeting Sec03Team05 Sprint04.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547076\Desktop\FreebiesforNewbies\Project_Files\GDP-02-Sprint05\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nwmissouri-my.sharepoint.com/personal/s546981_nwmissouri_edu/Documents/Documents/GitHub/FreebiesforNewbies/Project_Files/GDP-02-Sprint05/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71DEE1D-2127-415D-96A0-9C7AF9417E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{A71DEE1D-2127-415D-96A0-9C7AF9417E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5D8C02E-A810-40A0-BB42-F2E299913499}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Daily Stand-up Meeting Report</t>
   </si>
@@ -138,6 +138,24 @@
   </si>
   <si>
     <t>We are planning to complete the queries for Free Items Page</t>
+  </si>
+  <si>
+    <t>Created activities for Free items</t>
+  </si>
+  <si>
+    <t>Developing free items activities according to the requirements</t>
+  </si>
+  <si>
+    <t>Developed activities for create free item</t>
+  </si>
+  <si>
+    <t>Integrating UI with backend</t>
+  </si>
+  <si>
+    <t>Integrated and done with testing for free item activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preparing slides for midterm </t>
   </si>
 </sst>
 </file>
@@ -505,6 +523,11 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -537,11 +560,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -771,14 +789,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="23"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -801,12 +819,12 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A2" s="16"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="17"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="20"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -829,14 +847,14 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -859,14 +877,14 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="24"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="27"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -889,14 +907,14 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="24"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="27"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -981,7 +999,7 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="29" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="4"/>
@@ -1011,7 +1029,7 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A9" s="27"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1039,7 +1057,7 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A10" s="28"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -1067,7 +1085,7 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="5"/>
@@ -1097,7 +1115,7 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A12" s="10"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1125,7 +1143,7 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A13" s="11"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -1153,7 +1171,7 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="4"/>
@@ -1183,7 +1201,7 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A15" s="10"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="4"/>
       <c r="C15" s="6"/>
       <c r="D15" s="4"/>
@@ -1211,7 +1229,7 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A16" s="11"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1239,12 +1257,18 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="B17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1269,10 +1293,16 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A18" s="10"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -1297,10 +1327,16 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A19" s="11"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -1325,16 +1361,16 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="C20" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="10" t="s">
         <v>19</v>
       </c>
       <c r="E20" s="1"/>
@@ -1361,14 +1397,14 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A21" s="10"/>
-      <c r="B21" s="29" t="s">
+      <c r="A21" s="13"/>
+      <c r="B21" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="30" t="s">
+      <c r="C21" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="11" t="s">
         <v>20</v>
       </c>
       <c r="E21" s="1"/>
@@ -1395,14 +1431,14 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A22" s="11"/>
-      <c r="B22" s="30" t="s">
+      <c r="A22" s="14"/>
+      <c r="B22" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="30" t="s">
+      <c r="C22" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="30" t="s">
+      <c r="D22" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="1"/>
@@ -1515,10 +1551,10 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="13"/>
+      <c r="B26" s="16"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1545,8 +1581,8 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A27" s="14"/>
-      <c r="B27" s="15"/>
+      <c r="A27" s="17"/>
+      <c r="B27" s="18"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1573,8 +1609,8 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A28" s="16"/>
-      <c r="B28" s="17"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="20"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>

</xml_diff>